<commit_message>
Update import registration result - beta 3
Related Work Items: #949
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_K2 CNTT.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_K2 CNTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\StudyProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD928C6-2EE7-471A-88FA-F2824152A33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5730FB0-3ECC-4893-A0D6-5AD1653C43C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F19609F9-09B6-411B-92AB-95674FF34470}"/>
   </bookViews>
@@ -1618,7 +1618,7 @@
   <dimension ref="B1:S79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,7 +2689,9 @@
         <v>265</v>
       </c>
       <c r="R23" s="7"/>
-      <c r="S23" s="17"/>
+      <c r="S23" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" s="16"/>
@@ -2731,7 +2733,9 @@
         <v>265</v>
       </c>
       <c r="R24" s="7"/>
-      <c r="S24" s="17"/>
+      <c r="S24" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
@@ -2773,7 +2777,9 @@
         <v>265</v>
       </c>
       <c r="R25" s="7"/>
-      <c r="S25" s="17"/>
+      <c r="S25" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B26" s="16"/>

</xml_diff>